<commit_message>
Add score analysis for 1f and 5f
</commit_message>
<xml_diff>
--- a/health/scores/folds_3f.xlsx
+++ b/health/scores/folds_3f.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="16">
   <si>
     <t xml:space="preserve">FID</t>
   </si>
@@ -59,7 +59,16 @@
     <t xml:space="preserve">E(X)</t>
   </si>
   <si>
+    <t xml:space="preserve">Var(X)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">StDev(X)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Pred12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2StDev</t>
   </si>
   <si>
     <t xml:space="preserve">%Imp</t>
@@ -184,15 +193,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I114"/>
+  <dimension ref="A1:M114"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L7" activeCellId="0" sqref="L7"/>
+      <selection pane="topLeft" activeCell="I20" activeCellId="0" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="6" min="1" style="0" width="13.75"/>
+    <col collapsed="false" hidden="false" max="6" min="1" style="0" width="9.58673469387755"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
@@ -353,6 +362,20 @@
         <f aca="false">I5*I4</f>
         <v>2.54867256637168</v>
       </c>
+      <c r="J6" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="K6" s="0" t="n">
+        <f aca="false">(I3/I2)*(1 - (I3/I2))*I5*((I2-I5)/(I2-1))</f>
+        <v>1.81020999518924</v>
+      </c>
+      <c r="L6" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="M6" s="0" t="n">
+        <f aca="false">SQRT(K6)</f>
+        <v>1.3454404465413</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
@@ -375,12 +398,19 @@
         <v>0</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="I7" s="0" t="n">
         <f aca="false">COUNTIF(F2:F13, "=1")</f>
         <v>7</v>
       </c>
+      <c r="L7" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="M7" s="0" t="n">
+        <f aca="false">I6+2*M6</f>
+        <v>5.23955345945427</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
@@ -424,7 +454,7 @@
         <v>1</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I9" s="2" t="n">
         <f aca="false">I7/I6 - 1</f>
@@ -2652,10 +2682,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I114"/>
+  <dimension ref="A1:M114"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A79" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J10" activeCellId="0" sqref="J10"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J6" activeCellId="0" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -2820,6 +2850,20 @@
         <f aca="false">I5*I4</f>
         <v>2.44247787610619</v>
       </c>
+      <c r="J6" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="K6" s="0" t="n">
+        <f aca="false">(I3/I2)*(1 - (I3/I2))*I5*((I2-I5)/(I2-1))</f>
+        <v>1.75427654028171</v>
+      </c>
+      <c r="L6" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="M6" s="0" t="n">
+        <f aca="false">SQRT(K6)</f>
+        <v>1.32449104952873</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
@@ -2842,12 +2886,19 @@
         <v>0</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="I7" s="0" t="n">
         <f aca="false">COUNTIF(F2:F13, "=1")</f>
         <v>5</v>
       </c>
+      <c r="L7" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="M7" s="0" t="n">
+        <f aca="false">I6+2*M6</f>
+        <v>5.09145997516365</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
@@ -2891,7 +2942,7 @@
         <v>1</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I9" s="2" t="n">
         <f aca="false">I7/I6 - 1</f>
@@ -5119,10 +5170,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I114"/>
+  <dimension ref="A1:M114"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A85" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J6" activeCellId="0" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -5287,6 +5338,20 @@
         <f aca="false">I5*I4</f>
         <v>1.69911504424779</v>
       </c>
+      <c r="J6" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="K6" s="0" t="n">
+        <f aca="false">(I3/I2)*(1 - (I3/I2))*I5*((I2-I5)/(I2-1))</f>
+        <v>1.31528366691653</v>
+      </c>
+      <c r="L6" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="M6" s="0" t="n">
+        <f aca="false">SQRT(K6)</f>
+        <v>1.14685817210173</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
@@ -5309,12 +5374,19 @@
         <v>0</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="I7" s="0" t="n">
         <f aca="false">COUNTIF(F2:F13, "=1")</f>
         <v>4</v>
       </c>
+      <c r="L7" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="M7" s="0" t="n">
+        <f aca="false">I6+2*M6</f>
+        <v>3.99283138845125</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
@@ -5358,7 +5430,7 @@
         <v>1</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I9" s="2" t="n">
         <f aca="false">I7/I6 - 1</f>
@@ -7586,10 +7658,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I114"/>
+  <dimension ref="A1:M114"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
+      <selection pane="topLeft" activeCell="J6" activeCellId="0" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -7754,6 +7826,20 @@
         <f aca="false">I5*I4</f>
         <v>2.65486725663717</v>
       </c>
+      <c r="J6" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="K6" s="0" t="n">
+        <f aca="false">(I3/I2)*(1 - (I3/I2))*I5*((I2-I5)/(I2-1))</f>
+        <v>1.86444849691776</v>
+      </c>
+      <c r="L6" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="M6" s="0" t="n">
+        <f aca="false">SQRT(K6)</f>
+        <v>1.3654480938204</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
@@ -7776,12 +7862,19 @@
         <v>1</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="I7" s="0" t="n">
         <f aca="false">COUNTIF(F2:F13, "=1")</f>
         <v>6</v>
       </c>
+      <c r="L7" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="M7" s="0" t="n">
+        <f aca="false">I6+2*M6</f>
+        <v>5.38576344427796</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
@@ -7825,7 +7918,7 @@
         <v>1</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I9" s="2" t="n">
         <f aca="false">I7/I6 - 1</f>
@@ -10053,10 +10146,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I114"/>
+  <dimension ref="A1:M114"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J15" activeCellId="0" sqref="J15"/>
+      <selection pane="topLeft" activeCell="K10" activeCellId="0" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -10221,6 +10314,20 @@
         <f aca="false">I5*I4</f>
         <v>2.33628318584071</v>
       </c>
+      <c r="J6" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="K6" s="0" t="n">
+        <f aca="false">(I3/I2)*(1 - (I3/I2))*I5*((I2-I5)/(I2-1))</f>
+        <v>1.69664813219516</v>
+      </c>
+      <c r="L6" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="M6" s="0" t="n">
+        <f aca="false">SQRT(K6)</f>
+        <v>1.30255446419532</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
@@ -10243,12 +10350,19 @@
         <v>1</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="I7" s="0" t="n">
         <f aca="false">COUNTIF(F2:F13, "=1")</f>
         <v>5</v>
       </c>
+      <c r="L7" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="M7" s="0" t="n">
+        <f aca="false">I6+2*M6</f>
+        <v>4.94139211423135</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
@@ -10292,7 +10406,7 @@
         <v>1</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I9" s="2" t="n">
         <f aca="false">I7/I6 - 1</f>

</xml_diff>